<commit_message>
Added Delete code for deleting Posted data
</commit_message>
<xml_diff>
--- a/Data Files/LMSAPIHackathon.xlsx
+++ b/Data Files/LMSAPIHackathon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valli\Git\LMSRestAssuredAutomation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F368D23-201D-4F44-B8F0-FC045933EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322E2C5E-A451-4B8A-B995-B31127BED9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1416" yWindow="1020" windowWidth="21624" windowHeight="11220" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getsingleprogram" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="30">
   <si>
     <t>programId</t>
   </si>
@@ -113,73 +113,16 @@
     <t>SQL Bootcamp</t>
   </si>
   <si>
-    <t>null01</t>
-  </si>
-  <si>
-    <t>"1569"</t>
-  </si>
-  <si>
     <t>!@#</t>
   </si>
   <si>
     <t>!@#$</t>
   </si>
   <si>
-    <t>SQL100</t>
-  </si>
-  <si>
-    <t>SQL101</t>
-  </si>
-  <si>
-    <t>SQL102</t>
-  </si>
-  <si>
-    <t>sql 103</t>
-  </si>
-  <si>
-    <t>SQL105</t>
-  </si>
-  <si>
-    <t>SQL106</t>
-  </si>
-  <si>
-    <t>SQL107</t>
-  </si>
-  <si>
-    <t>SQL 105</t>
-  </si>
-  <si>
-    <t>SQL 106</t>
-  </si>
-  <si>
-    <t>SQL 107</t>
-  </si>
-  <si>
-    <t>SQL 108</t>
-  </si>
-  <si>
-    <t>SQL 109</t>
-  </si>
-  <si>
-    <t>SQL 110</t>
-  </si>
-  <si>
-    <t>SQL 111</t>
-  </si>
-  <si>
-    <t>SQL 112</t>
-  </si>
-  <si>
-    <t>SQL 113</t>
-  </si>
-  <si>
-    <t>SQL 114</t>
-  </si>
-  <si>
-    <t>SQL 115</t>
-  </si>
-  <si>
-    <t>SQL 116</t>
+    <t>SQL BootCamp527</t>
+  </si>
+  <si>
+    <t>"509"</t>
   </si>
 </sst>
 </file>
@@ -509,14 +452,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6D4306-2886-4BA4-8418-0C268B3307F2}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -539,7 +483,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -548,15 +492,12 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -565,12 +506,15 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -579,108 +523,108 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
       <c r="E8">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>24</v>
+      <c r="D9">
+        <v>-3</v>
       </c>
       <c r="E9">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10">
-        <v>-3</v>
-      </c>
-      <c r="E10">
-        <v>1569</v>
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -690,14 +634,11 @@
       </c>
       <c r="D11">
         <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -707,11 +648,14 @@
       </c>
       <c r="D12">
         <v>4</v>
+      </c>
+      <c r="E12">
+        <v>-509</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
@@ -722,13 +666,13 @@
       <c r="D13">
         <v>4</v>
       </c>
-      <c r="E13">
-        <v>-1569</v>
+      <c r="E13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -739,34 +683,17 @@
       <c r="D14">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
-        <v>24</v>
+      <c r="E14" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="5"/>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1" xr:uid="{CF4EDFE5-E42F-4500-B7BB-89B0B3D7520B}"/>
+    <hyperlink ref="E14" r:id="rId1" xr:uid="{CF4EDFE5-E42F-4500-B7BB-89B0B3D7520B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -798,7 +725,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -807,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +747,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -841,7 +768,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -850,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -863,7 +790,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -884,16 +811,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>1569</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -906,10 +833,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -927,7 +857,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -1108,7 +1038,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1143,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1177,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -1259,12 +1189,12 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <v>321</v>
+        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -1276,7 +1206,7 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <v>321</v>
+        <v>509</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -1284,7 +1214,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
@@ -1296,10 +1226,10 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>321</v>
+        <v>509</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1245,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29625D97-0824-478F-91BF-488D9AD8DBA8}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1338,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>321</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>